<commit_message>
Has working display with Text - Touch not working
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="51">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t xml:space="preserve">HELLO HAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is test</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1642,7 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
@@ -1656,7 +1659,7 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First commit to have Display & Touch working - YES
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="52">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">This is test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello IMR</t>
   </si>
 </sst>
 </file>
@@ -1642,7 +1645,7 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Add Splash Screen, MainMenu, and clickable AD Icon
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="61">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -171,6 +171,33 @@
   </si>
   <si>
     <t xml:space="preserve">Hello IMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iceland_45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iceland-Regular.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology Demonstrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog &amp; Digital</t>
   </si>
 </sst>
 </file>
@@ -1501,6 +1528,25 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1633,10 +1679,10 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
@@ -1645,15 +1691,15 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
@@ -1662,7 +1708,24 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds the AD and PA screen navigation to project Does not include anything happeing with AD screen
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="63">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">Analog &amp; Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM &amp; ACEL</t>
   </si>
 </sst>
 </file>
@@ -1728,6 +1734,23 @@
         <v>60</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Analog Digital Screen Working here. Some additions for the PWM Accelerometer screen are included but just started none of it does anything
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="98">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -204,6 +204,111 @@
   </si>
   <si>
     <t xml:space="preserve">PWM &amp; ACEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iceland_200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Digital_Read&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ADC_Read&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Analog_Read&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital_Dream_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital-dream.fat-skew.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital_Dream_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
   </si>
 </sst>
 </file>
@@ -1516,7 +1621,9 @@
         <v>17</v>
       </c>
       <c r="G6"/>
-      <c r="H6"/>
+      <c r="H6" t="s">
+        <v>80</v>
+      </c>
       <c r="I6"/>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -1549,9 +1656,13 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7"/>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
       <c r="H7"/>
-      <c r="I7"/>
+      <c r="I7" t="s">
+        <v>72</v>
+      </c>
       <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
@@ -1570,6 +1681,27 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1585,6 +1717,29 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1602,6 +1757,27 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10"/>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -1731,7 +1907,7 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1749,6 +1925,227 @@
       </c>
       <c r="F7" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Screen_PAPresenter is working. Includes Screen_AD previously working Merge to master and create a new branch from here
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="114">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -309,6 +309,54 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-00.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X:&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y:&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z:&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TILT</t>
   </si>
 </sst>
 </file>
@@ -1730,14 +1778,14 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="J9"/>
       <c r="L9" s="11" t="s">
@@ -2060,7 +2108,7 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
@@ -2077,7 +2125,7 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17">
@@ -2094,7 +2142,7 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18">
@@ -2111,7 +2159,7 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19">
@@ -2128,7 +2176,7 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20">
@@ -2145,7 +2193,75 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wifi Task Working and ready for pull request   Includes the ESP8266 Code for Wifi Access Point Operation   Task covers data exchange between websie and Tech Demo
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="130">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -357,6 +357,54 @@
   </si>
   <si>
     <t xml:space="preserve">TILT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WiFi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSID: IMR_TechDemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS: Connext123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPV4: 192.168.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONNECTION:</t>
   </si>
 </sst>
 </file>
@@ -2264,6 +2312,142 @@
         <v>113</v>
       </c>
     </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added Screen View, Music Queue, Timer 3
Not working is the FATFS.  It maybe an issues with CMSIS v1 vs v2
Will try going to v1
</commit_message>
<xml_diff>
--- a/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
+++ b/AppFirmware/TD_AppFirmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="132">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -405,6 +405,12 @@
   </si>
   <si>
     <t xml:space="preserve">CONNECTION:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUSIC</t>
   </si>
 </sst>
 </file>
@@ -2448,6 +2454,23 @@
         <v>129</v>
       </c>
     </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>